<commit_message>
Updated sample report spreadsheet.  See sort_value instructions for clarification.
</commit_message>
<xml_diff>
--- a/spreadsheet/sample_report.xlsx
+++ b/spreadsheet/sample_report.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wmg-my.sharepoint.com/personal/zachcox_elektra_com/Documents/elektra/interns/2019_summer/interview_test/spreadsheet/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3B98C03-A550-7E4B-8386-96DE96E5B483}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="127">
   <si>
     <t>artist</t>
   </si>
@@ -43,6 +37,9 @@
     <t>country</t>
   </si>
   <si>
+    <t>chart_type</t>
+  </si>
+  <si>
     <t>latest_pos</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
     <t>hist_pos</t>
   </si>
   <si>
+    <t>uri</t>
+  </si>
+  <si>
     <t>Jarrad Wright</t>
   </si>
   <si>
@@ -82,18 +82,18 @@
     <t>Cadet, Deno</t>
   </si>
   <si>
+    <t>Paulo Londra</t>
+  </si>
+  <si>
     <t>CXLOE</t>
   </si>
   <si>
-    <t>Paulo Londra</t>
+    <t>Ty James, Unheard</t>
   </si>
   <si>
     <t>Vincent</t>
   </si>
   <si>
-    <t>Ty James, Unheard</t>
-  </si>
-  <si>
     <t>Felix Cartal, LIGHTS</t>
   </si>
   <si>
@@ -118,18 +118,18 @@
     <t>Advice</t>
   </si>
   <si>
+    <t>Adan y Eva</t>
+  </si>
+  <si>
     <t>I Can't Have Nice Things</t>
   </si>
   <si>
-    <t>Adan y Eva</t>
+    <t>Splash</t>
   </si>
   <si>
     <t>Breathe 2.0</t>
   </si>
   <si>
-    <t>Splash</t>
-  </si>
-  <si>
     <t>Love Me</t>
   </si>
   <si>
@@ -154,12 +154,12 @@
     <t>2018-09-14</t>
   </si>
   <si>
+    <t>2018-11-05</t>
+  </si>
+  <si>
     <t>2019-02-15</t>
   </si>
   <si>
-    <t>2018-11-05</t>
-  </si>
-  <si>
     <t>2019-02-01</t>
   </si>
   <si>
@@ -184,18 +184,18 @@
     <t>Underrated Legends</t>
   </si>
   <si>
+    <t>WEA Latina</t>
+  </si>
+  <si>
     <t>EX EX / YOUNG&amp;VICIOUS</t>
   </si>
   <si>
-    <t>WEA Latina</t>
+    <t>Loyalty Records / Human Re Sources</t>
   </si>
   <si>
     <t>ICONS Music</t>
   </si>
   <si>
-    <t>Loyalty Records / Human Re Sources</t>
-  </si>
-  <si>
     <t>Physical Presents / Fontana North</t>
   </si>
   <si>
@@ -205,7 +205,7 @@
     <t>[45]</t>
   </si>
   <si>
-    <t>[57]</t>
+    <t>[56]</t>
   </si>
   <si>
     <t>[64]</t>
@@ -217,21 +217,21 @@
     <t>[73]</t>
   </si>
   <si>
-    <t>[68, 66]</t>
-  </si>
-  <si>
-    <t>[54]</t>
+    <t>[67, 66]</t>
   </si>
   <si>
     <t>[86]</t>
   </si>
   <si>
+    <t>[53]</t>
+  </si>
+  <si>
+    <t>[58, 58]</t>
+  </si>
+  <si>
     <t>[55]</t>
   </si>
   <si>
-    <t>[58, 58]</t>
-  </si>
-  <si>
     <t>[66, 63]</t>
   </si>
   <si>
@@ -259,6 +259,12 @@
     <t>United States</t>
   </si>
   <si>
+    <t>viral</t>
+  </si>
+  <si>
+    <t>regional</t>
+  </si>
+  <si>
     <t>2019-03-15</t>
   </si>
   <si>
@@ -274,21 +280,21 @@
     <t>2019-03-16</t>
   </si>
   <si>
+    <t>2019-02-08</t>
+  </si>
+  <si>
     <t>2019-03-13</t>
   </si>
   <si>
-    <t>2019-02-08</t>
-  </si>
-  <si>
     <t>2019-03-08</t>
   </si>
   <si>
+    <t>2018-12-28</t>
+  </si>
+  <si>
     <t>2019-03-10</t>
   </si>
   <si>
-    <t>2018-12-28</t>
-  </si>
-  <si>
     <t>2019-02-26</t>
   </si>
   <si>
@@ -322,12 +328,12 @@
     <t>38, 39, 29, 28, 28, 24, 25, 26, 17, 19, 20, 9, 8, 6, 4, 4, 3, 3, 3, 5, 5, 7, 7, 9, 9, 7, 8, 6, 6, 6, 6, 6, 6, 10, 9, 7, 7, 7, 8, 6, 11, 12, 16, 16, 12, 11, 12, 25, 23, 17, 19, 19, 20, 21, 22, 23, 29, 28, 23, 25, 30</t>
   </si>
   <si>
+    <t>165, 124, 117, 126, 110, 112, 104, 91, 92, 92, 93, 83, 83, 80, 70, 67, 65, 63, 68, 65, 64, 58, 56, 53, 51, 54, 57, 57, 56, 51, 51, 50, 56, 47, 48, 45, 45, 42, 45, 41, 39, 43, 40, 39, 41, 40, 41, 40, 45, 45, 45, 45, 45, 49, 46, 47, 47, 43, 44, 44, 48, 41, 48, 43, 40, 40, 42, 40, 38, 38, 42, 43, 52, 51, 63, 80, 91, 68, 65, 65, 70, 79, 86, 97, 68, 64, 63, 64, 69, 78, 84, 65, 66, 66, 74, 81, 89, 99, 129, 45, 46, 43, 46, 66, 59, 51, 54, 63, 54, 55, 56, 52, 53, 53, 53, 51, 55, 52, 50, 47, 47, 49, 46, 51, 45, 47, 46, 47, 45, 47, 51, 47, 49, 49, 50, 52, 49, 53, 50, 50, 48, 49, 73, 21, 24, 22, 24, 24, 22, 21, 22, 22, 23, 24, 26, 22, 21, 21, 21, 22, 22, 22, 23, 24, 24, 23, 24, 23, 22, 35, 29, 31, 31, 31, 31, 30, 30, 29, 32, 31</t>
+  </si>
+  <si>
     <t>39, 35, 47, 45, 37, 43, 38, 36, 33, 37, 35, 32, 27, 29, 35, 31</t>
   </si>
   <si>
-    <t>165, 124, 117, 126, 110, 112, 104, 91, 92, 92, 93, 83, 83, 80, 70, 67, 65, 63, 68, 65, 64, 58, 56, 53, 51, 54, 57, 57, 56, 51, 51, 50, 56, 47, 48, 45, 45, 42, 45, 41, 39, 43, 40, 39, 41, 40, 41, 40, 45, 45, 45, 45, 45, 49, 46, 47, 47, 43, 44, 44, 48, 41, 48, 43, 40, 40, 42, 40, 38, 38, 42, 43, 52, 51, 63, 80, 91, 68, 65, 65, 70, 79, 86, 97, 68, 64, 63, 64, 69, 78, 84, 65, 66, 66, 74, 81, 89, 99, 129, 45, 46, 43, 46, 66, 59, 51, 54, 63, 54, 55, 56, 52, 53, 53, 53, 51, 55, 52, 50, 47, 47, 49, 46, 51, 45, 47, 46, 47, 45, 47, 51, 47, 49, 49, 50, 52, 49, 53, 50, 50, 48, 49, 73, 21, 24, 22, 24, 24, 22, 21, 22, 22, 23, 24, 26, 22, 21, 21, 21, 22, 22, 22, 23, 24, 24, 23, 24, 23, 22, 35, 29, 31, 31, 31, 31, 30, 30, 29, 32, 31</t>
-  </si>
-  <si>
     <t>50, 43, 41, 42, 42, 41, 44, 43, 43, 40, 31, 26, 26, 30, 30, 29, 27, 27, 29, 32</t>
   </si>
   <si>
@@ -337,18 +343,18 @@
     <t>42, 41, 40, 41, 45, 44, 44, 48, 49, 35, 34, 32, 35</t>
   </si>
   <si>
+    <t>132, 132, 83, 61, 58, 58, 51, 46, 41, 35, 33, 24, 22, 20, 18, 18, 16, 14, 14, 15, 15, 15, 20, 19, 18, 14, 15, 16, 13, 11, 11, 18, 14, 17, 14, 13, 13, 13, 14, 14, 15, 15, 14, 14, 13, 16, 16, 19, 41, 45, 11, 12, 11, 10, 11, 11, 11, 14, 14, 14, 12, 12, 15, 14, 14, 14, 15, 12, 12, 15, 15, 15, 15, 15, 12, 13, 13, 13, 14, 15, 14, 12, 12, 16, 17, 17, 16, 16, 16, 16, 17, 19, 19, 19, 32, 28, 30, 32, 32, 31, 28, 28, 21, 19, 27, 24, 27, 26, 24, 21, 23, 30, 30, 30, 27, 29, 27, 27, 31, 32, 33, 33, 36, 32, 33, 34, 34, 36, 35, 32, 28, 37</t>
+  </si>
+  <si>
     <t>34, 34, 35, 46, 46, 44, 37</t>
   </si>
   <si>
-    <t>132, 132, 83, 61, 58, 58, 51, 46, 41, 35, 33, 24, 22, 20, 18, 18, 16, 14, 14, 15, 15, 15, 20, 19, 18, 14, 15, 16, 13, 11, 11, 18, 14, 17, 14, 13, 13, 13, 14, 14, 15, 15, 14, 14, 13, 16, 16, 19, 41, 45, 11, 12, 11, 10, 11, 11, 11, 14, 14, 14, 12, 12, 15, 14, 14, 14, 15, 12, 12, 15, 15, 15, 15, 15, 12, 13, 13, 13, 14, 15, 14, 12, 12, 16, 17, 17, 16, 16, 16, 16, 17, 19, 19, 19, 32, 28, 30, 32, 32, 31, 28, 28, 21, 19, 27, 24, 27, 26, 24, 21, 23, 30, 30, 30, 27, 29, 27, 27, 31, 32, 33, 33, 36, 32, 33, 34, 34, 36, 35, 32, 28, 37</t>
+    <t>21, 20, 17, 18, 20, 22, 19, 26, 27, 27, 26, 24, 23, 24, 37, 34, 34, 33, 34, 35, 39</t>
   </si>
   <si>
     <t>47, 41, 47, 39</t>
   </si>
   <si>
-    <t>21, 20, 17, 18, 20, 22, 19, 26, 27, 27, 26, 24, 23, 24, 37, 34, 34, 33, 34, 35, 39</t>
-  </si>
-  <si>
     <t>49, 46, 40, 39, 40</t>
   </si>
   <si>
@@ -373,32 +379,29 @@
     <t>spotify:track:1fp2uoWXPca3mIdxRHIgQm</t>
   </si>
   <si>
+    <t>spotify:track:6FyRXC8tJUh863JCkyWqtk</t>
+  </si>
+  <si>
     <t>spotify:track:4CnBuBzStNaCMuX6UlA7LB</t>
   </si>
   <si>
-    <t>spotify:track:6FyRXC8tJUh863JCkyWqtk</t>
+    <t>spotify:track:1LIPyl9jbqlf7vBfTOFeoB</t>
   </si>
   <si>
     <t>spotify:track:4aZLKRZLXeSLcFtp7H3PgI</t>
   </si>
   <si>
-    <t>spotify:track:1LIPyl9jbqlf7vBfTOFeoB</t>
-  </si>
-  <si>
     <t>spotify:track:53hNIcq8OLj9OUNvQ4ulFM</t>
   </si>
   <si>
     <t>spotify:track:0bLcyYNAPLh6oQTGnRxvSC</t>
-  </si>
-  <si>
-    <t>track_uri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,14 +464,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -515,7 +510,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,27 +542,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -599,24 +576,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -792,16 +751,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -845,1007 +802,1070 @@
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2">
+        <v>74</v>
+      </c>
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2">
         <v>4</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>7</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>2</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>4</v>
       </c>
-      <c r="M2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2">
+      <c r="N2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
-        <v>91</v>
-      </c>
       <c r="P2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F3">
         <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3">
+        <v>75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3">
         <v>9</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>10</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>2</v>
       </c>
-      <c r="M3" t="s">
-        <v>80</v>
-      </c>
-      <c r="N3">
+      <c r="N3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O3">
         <v>-1</v>
       </c>
-      <c r="O3" t="s">
-        <v>92</v>
-      </c>
       <c r="P3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4">
+        <v>75</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4">
         <v>10</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>14</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>8</v>
       </c>
-      <c r="M4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N4">
+      <c r="N4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4">
         <v>-1</v>
       </c>
-      <c r="O4" t="s">
-        <v>93</v>
-      </c>
       <c r="P4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5">
         <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I5">
+        <v>76</v>
+      </c>
+      <c r="I5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5">
         <v>11</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>84</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>4</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>8</v>
       </c>
-      <c r="M5" t="s">
-        <v>82</v>
-      </c>
-      <c r="N5">
+      <c r="N5" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5">
         <v>0</v>
       </c>
-      <c r="O5" t="s">
-        <v>94</v>
-      </c>
       <c r="P5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F6">
         <v>81</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I6">
+        <v>76</v>
+      </c>
+      <c r="I6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6">
         <v>13</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>72</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>4</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="M6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6">
+      <c r="N6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6">
         <v>-1</v>
       </c>
-      <c r="O6" t="s">
-        <v>95</v>
-      </c>
       <c r="P6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I7">
+        <v>77</v>
+      </c>
+      <c r="I7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7">
         <v>15</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>7</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>2</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>9</v>
       </c>
-      <c r="M7" t="s">
-        <v>81</v>
-      </c>
-      <c r="N7">
+      <c r="N7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7">
         <v>-2</v>
       </c>
-      <c r="O7" t="s">
-        <v>96</v>
-      </c>
       <c r="P7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F8">
         <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8">
+        <v>78</v>
+      </c>
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8">
         <v>23</v>
-      </c>
-      <c r="J8">
-        <v>6</v>
       </c>
       <c r="K8">
         <v>6</v>
       </c>
       <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
         <v>23</v>
       </c>
-      <c r="M8" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8">
+      <c r="N8" t="s">
+        <v>87</v>
+      </c>
+      <c r="O8">
         <v>5</v>
       </c>
-      <c r="O8" t="s">
-        <v>97</v>
-      </c>
       <c r="P8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F9">
         <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9">
+        <v>77</v>
+      </c>
+      <c r="I9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9">
         <v>28</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>12</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>6</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>28</v>
       </c>
-      <c r="M9" t="s">
-        <v>83</v>
-      </c>
-      <c r="N9">
+      <c r="N9" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9">
         <v>4</v>
       </c>
-      <c r="O9" t="s">
-        <v>98</v>
-      </c>
       <c r="P9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F10">
         <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10">
+        <v>78</v>
+      </c>
+      <c r="I10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10">
         <v>30</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>61</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>4</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>3</v>
       </c>
-      <c r="M10" t="s">
-        <v>82</v>
-      </c>
-      <c r="N10">
+      <c r="N10" t="s">
+        <v>86</v>
+      </c>
+      <c r="O10">
         <v>-5</v>
       </c>
-      <c r="O10" t="s">
-        <v>99</v>
-      </c>
       <c r="P10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F11">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11">
         <v>31</v>
       </c>
-      <c r="J11">
-        <v>16</v>
-      </c>
       <c r="K11">
-        <v>6</v>
+        <v>180</v>
       </c>
       <c r="L11">
-        <v>27</v>
-      </c>
-      <c r="M11" t="s">
-        <v>84</v>
-      </c>
-      <c r="N11">
-        <v>4</v>
-      </c>
-      <c r="O11" t="s">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>88</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12">
+        <v>73</v>
+      </c>
+      <c r="G12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12">
-        <v>77</v>
-      </c>
-      <c r="G12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" t="s">
-        <v>74</v>
-      </c>
-      <c r="I12">
-        <v>31</v>
-      </c>
-      <c r="J12">
-        <v>180</v>
-      </c>
       <c r="K12">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="L12">
-        <v>21</v>
-      </c>
-      <c r="M12" t="s">
-        <v>85</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12" t="s">
-        <v>101</v>
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>27</v>
+      </c>
+      <c r="N12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
       </c>
       <c r="P12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F13">
         <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13">
+        <v>80</v>
+      </c>
+      <c r="I13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13">
         <v>32</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>20</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>6</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>26</v>
       </c>
-      <c r="M13" t="s">
-        <v>86</v>
-      </c>
-      <c r="N13">
+      <c r="N13" t="s">
+        <v>90</v>
+      </c>
+      <c r="O13">
         <v>-3</v>
       </c>
-      <c r="O13" t="s">
-        <v>102</v>
-      </c>
       <c r="P13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F14">
         <v>73</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
-      </c>
-      <c r="I14">
+        <v>76</v>
+      </c>
+      <c r="I14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14">
         <v>34</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>17</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>6</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>34</v>
       </c>
-      <c r="M14" t="s">
-        <v>83</v>
-      </c>
-      <c r="N14">
+      <c r="N14" t="s">
+        <v>87</v>
+      </c>
+      <c r="O14">
         <v>1</v>
       </c>
-      <c r="O14" t="s">
-        <v>103</v>
-      </c>
       <c r="P14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F15">
         <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15">
+        <v>74</v>
+      </c>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15">
         <v>35</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>13</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>6</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>32</v>
       </c>
-      <c r="M15" t="s">
-        <v>79</v>
-      </c>
-      <c r="N15">
+      <c r="N15" t="s">
+        <v>83</v>
+      </c>
+      <c r="O15">
         <v>-3</v>
       </c>
-      <c r="O15" t="s">
-        <v>104</v>
-      </c>
       <c r="P15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F16">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16">
+        <v>75</v>
+      </c>
+      <c r="I16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16">
         <v>37</v>
       </c>
-      <c r="J16">
-        <v>7</v>
-      </c>
       <c r="K16">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="L16">
-        <v>34</v>
-      </c>
-      <c r="M16" t="s">
-        <v>87</v>
-      </c>
-      <c r="N16">
-        <v>7</v>
-      </c>
-      <c r="O16" t="s">
-        <v>105</v>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16" t="s">
+        <v>91</v>
+      </c>
+      <c r="O16">
+        <v>-9</v>
       </c>
       <c r="P16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F17">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17">
+        <v>74</v>
+      </c>
+      <c r="I17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17">
         <v>37</v>
       </c>
-      <c r="J17">
-        <v>132</v>
-      </c>
       <c r="K17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="L17">
-        <v>10</v>
-      </c>
-      <c r="M17" t="s">
-        <v>88</v>
-      </c>
-      <c r="N17">
-        <v>-9</v>
-      </c>
-      <c r="O17" t="s">
-        <v>106</v>
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>34</v>
+      </c>
+      <c r="N17" t="s">
+        <v>92</v>
+      </c>
+      <c r="O17">
+        <v>7</v>
       </c>
       <c r="P17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F18">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H18" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18">
+        <v>80</v>
+      </c>
+      <c r="I18" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18">
         <v>39</v>
       </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
       <c r="K18">
+        <v>21</v>
+      </c>
+      <c r="L18">
         <v>1</v>
       </c>
-      <c r="L18">
-        <v>39</v>
-      </c>
-      <c r="M18" t="s">
-        <v>83</v>
-      </c>
-      <c r="N18">
-        <v>8</v>
-      </c>
-      <c r="O18" t="s">
-        <v>107</v>
+      <c r="M18">
+        <v>17</v>
+      </c>
+      <c r="N18" t="s">
+        <v>93</v>
+      </c>
+      <c r="O18">
+        <v>-4</v>
       </c>
       <c r="P18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F19">
+        <v>52</v>
+      </c>
+      <c r="G19" t="s">
         <v>71</v>
       </c>
-      <c r="G19" t="s">
-        <v>69</v>
-      </c>
       <c r="H19" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19">
+        <v>74</v>
+      </c>
+      <c r="I19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19">
         <v>39</v>
       </c>
-      <c r="J19">
-        <v>21</v>
-      </c>
       <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
         <v>1</v>
       </c>
-      <c r="L19">
-        <v>17</v>
-      </c>
-      <c r="M19" t="s">
-        <v>89</v>
-      </c>
-      <c r="N19">
-        <v>-4</v>
-      </c>
-      <c r="O19" t="s">
-        <v>108</v>
+      <c r="M19">
+        <v>39</v>
+      </c>
+      <c r="N19" t="s">
+        <v>87</v>
+      </c>
+      <c r="O19">
+        <v>8</v>
       </c>
       <c r="P19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F20">
         <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
-      </c>
-      <c r="I20">
+        <v>79</v>
+      </c>
+      <c r="I20" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20">
         <v>40</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>5</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>1</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>39</v>
       </c>
-      <c r="M20" t="s">
-        <v>79</v>
-      </c>
-      <c r="N20">
+      <c r="N20" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20">
         <v>-1</v>
       </c>
-      <c r="O20" t="s">
-        <v>109</v>
-      </c>
       <c r="P20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F21">
         <v>57</v>
       </c>
       <c r="G21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21">
+        <v>79</v>
+      </c>
+      <c r="I21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21">
         <v>45</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>10</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>1</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>36</v>
       </c>
-      <c r="M21" t="s">
-        <v>90</v>
-      </c>
-      <c r="N21">
+      <c r="N21" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21">
         <v>4</v>
       </c>
-      <c r="O21" t="s">
-        <v>110</v>
-      </c>
       <c r="P21" t="s">
-        <v>122</v>
+        <v>114</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>